<commit_message>
Started base class development
</commit_message>
<xml_diff>
--- a/zzz/SQLite Options.xlsx
+++ b/zzz/SQLite Options.xlsx
@@ -42,9 +42,6 @@
     <t>No</t>
   </si>
   <si>
-    <t>Setting is persistent (stored in database file)</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -322,6 +319,9 @@
   </si>
   <si>
     <t>Apply to existing databases?</t>
+  </si>
+  <si>
+    <t>Persistent (stored in database file)</t>
   </si>
 </sst>
 </file>
@@ -690,7 +690,7 @@
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -706,12 +706,12 @@
     <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="71.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>1</v>
@@ -720,27 +720,27 @@
         <v>2</v>
       </c>
       <c r="E1" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="F1" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>7</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>4</v>
@@ -749,91 +749,91 @@
         <v>6</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="C4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -841,233 +841,233 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>55</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C8" s="4" t="s">
+      <c r="D8" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>41</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>95</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>44</v>
-      </c>
       <c r="D10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="4" t="s">
+      <c r="D11" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="4" t="s">
+      <c r="D12" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="E12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="4" t="s">
+      <c r="D13" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>83</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1075,50 +1075,50 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B19" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="E19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="G19" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>6</v>
@@ -1127,137 +1127,137 @@
         <v>6</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D21" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H21" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D22" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H22" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C23" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="E23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H23" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D24" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H24" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C25" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="E25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H25" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
First version of DatabaseHandler
</commit_message>
<xml_diff>
--- a/zzz/SQLite Options.xlsx
+++ b/zzz/SQLite Options.xlsx
@@ -126,9 +126,6 @@
     <t>(None)</t>
   </si>
   <si>
-    <t xml:space="preserve">Can only be changed when the database is empty (before the first CREATE TABLE statement. Min=256, Max=65536 </t>
-  </si>
-  <si>
     <t>Legacy Format=True/False</t>
   </si>
   <si>
@@ -334,6 +331,9 @@
   </si>
   <si>
     <t>Returns the SQLite version. Can not be set.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can only be changed when the database is empty (before the first CREATE TABLE statement. Min=512, Max=65536 </t>
   </si>
 </sst>
 </file>
@@ -702,7 +702,7 @@
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -732,13 +732,13 @@
         <v>2</v>
       </c>
       <c r="E1" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>97</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>98</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>7</v>
@@ -746,7 +746,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>3</v>
@@ -793,7 +793,7 @@
         <v>12</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -819,7 +819,7 @@
         <v>6</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -856,7 +856,7 @@
         <v>30</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>31</v>
@@ -871,21 +871,21 @@
         <v>12</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>35</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>53</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>6</v>
@@ -897,21 +897,21 @@
         <v>12</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" s="4" t="s">
+      <c r="D8" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>6</v>
@@ -923,21 +923,21 @@
         <v>17</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>92</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>6</v>
@@ -949,21 +949,21 @@
         <v>12</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>42</v>
-      </c>
       <c r="D10" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>12</v>
@@ -975,21 +975,21 @@
         <v>17</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>57</v>
-      </c>
       <c r="D11" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>17</v>
@@ -1001,47 +1001,47 @@
         <v>17</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="4" t="s">
+      <c r="D12" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="E12" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>67</v>
-      </c>
       <c r="D13" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>17</v>
@@ -1053,33 +1053,33 @@
         <v>17</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>81</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1087,12 +1087,12 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>15</v>
@@ -1113,12 +1113,12 @@
         <v>18</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>32</v>
@@ -1144,42 +1144,42 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D21" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H21" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>17</v>
@@ -1191,21 +1191,21 @@
         <v>17</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C23" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>70</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>17</v>
@@ -1217,85 +1217,85 @@
         <v>17</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D24" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H24" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C25" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="E25" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H25" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C26" s="4" t="s">
+      <c r="D26" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="E26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H26" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
DBOptionXXX is now feature complete
</commit_message>
<xml_diff>
--- a/zzz/SQLite Options.xlsx
+++ b/zzz/SQLite Options.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="106">
   <si>
     <t>Option Name</t>
   </si>
@@ -96,244 +96,247 @@
     <t>PRAGMA main.synchronous;</t>
   </si>
   <si>
+    <t xml:space="preserve">FULL is slow, but very safe. OFF is fast, but unsafe. </t>
+  </si>
+  <si>
+    <t>Page Size=(Bytes)</t>
+  </si>
+  <si>
+    <t>http://www.sqlite.org/pragma.html#pragma_page_size</t>
+  </si>
+  <si>
+    <t>Enlist=Y/N</t>
+  </si>
+  <si>
+    <t>Automatically enlist in distributed transactions (MSDTC)</t>
+  </si>
+  <si>
+    <t>(None)</t>
+  </si>
+  <si>
+    <t>Legacy Format=True/False</t>
+  </si>
+  <si>
+    <t>Journal Mode</t>
+  </si>
+  <si>
+    <t>PRAGMA main.journal_mode</t>
+  </si>
+  <si>
+    <t>http://www.sqlite.org/pragma.html#pragma_journal_mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRAGMA main.page_size; </t>
+  </si>
+  <si>
+    <t>Automatic Index</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRAGMA main.automatic_index; </t>
+  </si>
+  <si>
+    <t>Values: DELETE | TRUNCATE | PERSIST | MEMORY | WAL | OFF. See Link for full description. Can be applied to existing databases when VACUUM is used - for this program this is not used</t>
+  </si>
+  <si>
+    <t>Journal Mode=(Value)</t>
+  </si>
+  <si>
+    <t>http://www.sqlite.org/pragma.html#pragma_automatic_index</t>
+  </si>
+  <si>
+    <t>Yes/No. Controls if SQLite is allowed to create a temporary index to aid query a query</t>
+  </si>
+  <si>
+    <t>http://www.sqlite.org/pragma.html#pragma_cache_spill</t>
+  </si>
+  <si>
+    <t>"cache spilling is usually advantageous. However, a cache spill has the side-effect of acquiring an EXCLUSIVE lock on the database file. "</t>
+  </si>
+  <si>
+    <t>"True - Use the more compatible legacy 3.x database format; False - Use the newer 3.3x database format which compresses numbers more effectively "</t>
+  </si>
+  <si>
+    <t>http://www.sqlite.org/pragma.html#pragma_journal_size_limit</t>
+  </si>
+  <si>
+    <t>"The journal_size_limit pragma may be used to limit the size of rollback-journal and WAL files left in the file-system after transactions or checkpoints."</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRAGMA legacy_file_format; </t>
+  </si>
+  <si>
+    <t>http://www.sqlite.org/pragma.html#pragma_legacy_file_format</t>
+  </si>
+  <si>
+    <t>http://www.sqlite.org/pragma.html#pragma_locking_mode</t>
+  </si>
+  <si>
+    <t>Locking Mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRAGMA main.locking_mode; </t>
+  </si>
+  <si>
+    <t>NORMAL / EXCLUSIVE. Controls if exclusive mode is used or not.</t>
+  </si>
+  <si>
+    <t>PRAGMA main.secure_delete;</t>
+  </si>
+  <si>
+    <t>http://www.sqlite.org/pragma.html#pragma_secure_delete</t>
+  </si>
+  <si>
+    <t>Yes/No. Deleted data will be overwritten with zeros.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRAGMA [main].cache_spill; </t>
+  </si>
+  <si>
+    <t>PRAGMA main.journal_size_limit;</t>
+  </si>
+  <si>
+    <t>http://www.sqlite.org/pragma.html#pragma_temp_store</t>
+  </si>
+  <si>
+    <t>PRAGMA temp_store;</t>
+  </si>
+  <si>
+    <t>File/Memory. Defines where temporary tables and indices are stored.</t>
+  </si>
+  <si>
+    <t>PRAGMA threads;</t>
+  </si>
+  <si>
+    <t>http://www.sqlite.org/pragma.html#pragma_threads</t>
+  </si>
+  <si>
+    <t>"This limit sets an upper bound on the number of auxiliary threads that a prepared statement is allowed to launch to assist with a query. "</t>
+  </si>
+  <si>
+    <t>System.Data.SQLLite only allows UTF-8 or UTF-16le. Must be set using connection string when opening an Zero byte file to be applied.</t>
+  </si>
+  <si>
+    <t>http://www.sqlite.org/pragma.html#pragma_wal_checkpoint</t>
+  </si>
+  <si>
+    <t>This pragma causes a checkpoint operation to run, if WAL log is enabled.</t>
+  </si>
+  <si>
+    <t>PRAGMA wal_autocheckpoint;</t>
+  </si>
+  <si>
+    <t>http://www.sqlite.org/pragma.html#pragma_wal_autocheckpoint</t>
+  </si>
+  <si>
+    <t>"When the write-ahead log is enabled (via the journal_mode pragma) a checkpoint will be run automatically whenever the write-ahead log equals or exceeds N pages in length."</t>
+  </si>
+  <si>
+    <t>Positive value: Set cache to VALUE*page_size. Negative: Set cache directly to the value in kB (e.g. =-10 means 10 kB)</t>
+  </si>
+  <si>
+    <t>https://www.sqlite.org/lang_corefunc.html#sqlite_version</t>
+  </si>
+  <si>
+    <t>select sqlite_version();</t>
+  </si>
+  <si>
+    <t>?? BinaryGUID</t>
+  </si>
+  <si>
+    <t>?? Enlist</t>
+  </si>
+  <si>
+    <t>?? Cache Spill</t>
+  </si>
+  <si>
+    <t>?? Jounal Size Limit</t>
+  </si>
+  <si>
+    <t>?? Threads</t>
+  </si>
+  <si>
+    <t>?? WAL Checkpoint</t>
+  </si>
+  <si>
+    <t>?? WAL AutoCheckPoint</t>
+  </si>
+  <si>
+    <t>"True - Store GUID columns in binary form; False - Store GUID columns as text "</t>
+  </si>
+  <si>
+    <t>http://www.sqlite.org/pragma.html#pragma_auto_vacuum</t>
+  </si>
+  <si>
+    <t>None/Full. Can be changed for new databases only. Enabled a "Mini Vacuum" after deleting data. The value INCREMENTAL is not supported by this program.</t>
+  </si>
+  <si>
+    <t>PRAGMA main.auto_vacuum;</t>
+  </si>
+  <si>
+    <t>PRAGMA main.wal_checkpoint;</t>
+  </si>
+  <si>
+    <t>Is verifiable?</t>
+  </si>
+  <si>
+    <t>Apply to existing databases?</t>
+  </si>
+  <si>
+    <t>Persistent (stored in database file)</t>
+  </si>
+  <si>
+    <t>PRAGMA cell_size_check;</t>
+  </si>
+  <si>
+    <t>http://www.sqlite.org/pragma.html#pragma_cell_size_check</t>
+  </si>
+  <si>
+    <t>"The cell_size_check pragma enables or disables additional sanity checking on database b-tree pages as they are initially read from disk."</t>
+  </si>
+  <si>
+    <t>Returns the SQLite version. Can not be set.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can only be changed when the database is empty (before the first CREATE TABLE statement. Min=512, Max=65536 </t>
+  </si>
+  <si>
+    <t>?? LegacyFormat</t>
+  </si>
+  <si>
+    <t>Cell Size Check</t>
+  </si>
+  <si>
+    <t>?? In-Memory Database</t>
+  </si>
+  <si>
+    <t>?? Auto Vacuum</t>
+  </si>
+  <si>
+    <t>The following entries might also have an effect on performance but are not implemented by this program so far.</t>
+  </si>
+  <si>
+    <t>Depends</t>
+  </si>
+  <si>
+    <t>UTF-8 or UTF16le Encoding</t>
+  </si>
+  <si>
+    <t>Cache Size</t>
+  </si>
+  <si>
+    <t>Page Size</t>
+  </si>
+  <si>
     <t>Synchronous</t>
   </si>
   <si>
-    <t xml:space="preserve">FULL is slow, but very safe. OFF is fast, but unsafe. </t>
-  </si>
-  <si>
-    <t>Page Size=(Bytes)</t>
-  </si>
-  <si>
-    <t>http://www.sqlite.org/pragma.html#pragma_page_size</t>
-  </si>
-  <si>
-    <t>Enlist=Y/N</t>
-  </si>
-  <si>
-    <t>Automatically enlist in distributed transactions (MSDTC)</t>
-  </si>
-  <si>
-    <t>(None)</t>
-  </si>
-  <si>
-    <t>Legacy Format=True/False</t>
-  </si>
-  <si>
-    <t>Journal Mode</t>
-  </si>
-  <si>
-    <t>PRAGMA main.journal_mode</t>
-  </si>
-  <si>
-    <t>http://www.sqlite.org/pragma.html#pragma_journal_mode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRAGMA main.page_size; </t>
-  </si>
-  <si>
-    <t>Automatic Index</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRAGMA main.automatic_index; </t>
-  </si>
-  <si>
-    <t>Values: DELETE | TRUNCATE | PERSIST | MEMORY | WAL | OFF. See Link for full description. Can be applied to existing databases when VACUUM is used - for this program this is not used</t>
-  </si>
-  <si>
-    <t>Journal Mode=(Value)</t>
-  </si>
-  <si>
-    <t>http://www.sqlite.org/pragma.html#pragma_automatic_index</t>
-  </si>
-  <si>
-    <t>Yes/No. Controls if SQLite is allowed to create a temporary index to aid query a query</t>
-  </si>
-  <si>
-    <t>http://www.sqlite.org/pragma.html#pragma_cache_spill</t>
-  </si>
-  <si>
-    <t>"cache spilling is usually advantageous. However, a cache spill has the side-effect of acquiring an EXCLUSIVE lock on the database file. "</t>
-  </si>
-  <si>
-    <t>"True - Use the more compatible legacy 3.x database format; False - Use the newer 3.3x database format which compresses numbers more effectively "</t>
-  </si>
-  <si>
-    <t>http://www.sqlite.org/pragma.html#pragma_journal_size_limit</t>
-  </si>
-  <si>
-    <t>"The journal_size_limit pragma may be used to limit the size of rollback-journal and WAL files left in the file-system after transactions or checkpoints."</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRAGMA legacy_file_format; </t>
-  </si>
-  <si>
-    <t>http://www.sqlite.org/pragma.html#pragma_legacy_file_format</t>
-  </si>
-  <si>
-    <t>LegacyFormat</t>
-  </si>
-  <si>
-    <t>http://www.sqlite.org/pragma.html#pragma_locking_mode</t>
-  </si>
-  <si>
-    <t>Locking Mode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRAGMA main.locking_mode; </t>
-  </si>
-  <si>
-    <t>NORMAL / EXCLUSIVE. Controls if exclusive mode is used or not.</t>
-  </si>
-  <si>
-    <t>PRAGMA main.secure_delete;</t>
-  </si>
-  <si>
-    <t>http://www.sqlite.org/pragma.html#pragma_secure_delete</t>
-  </si>
-  <si>
-    <t>Yes/No. Deleted data will be overwritten with zeros.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRAGMA [main].cache_spill; </t>
-  </si>
-  <si>
-    <t>PRAGMA main.journal_size_limit;</t>
-  </si>
-  <si>
-    <t>http://www.sqlite.org/pragma.html#pragma_temp_store</t>
-  </si>
-  <si>
-    <t>PRAGMA temp_store;</t>
-  </si>
-  <si>
-    <t>File/Memory. Defines where temporary tables and indices are stored.</t>
-  </si>
-  <si>
-    <t>PRAGMA threads;</t>
-  </si>
-  <si>
-    <t>http://www.sqlite.org/pragma.html#pragma_threads</t>
-  </si>
-  <si>
-    <t>"This limit sets an upper bound on the number of auxiliary threads that a prepared statement is allowed to launch to assist with a query. "</t>
-  </si>
-  <si>
-    <t>System.Data.SQLLite only allows UTF-8 or UTF-16le. Must be set using connection string when opening an Zero byte file to be applied.</t>
-  </si>
-  <si>
-    <t>http://www.sqlite.org/pragma.html#pragma_wal_checkpoint</t>
-  </si>
-  <si>
-    <t>This pragma causes a checkpoint operation to run, if WAL log is enabled.</t>
-  </si>
-  <si>
-    <t>PRAGMA wal_autocheckpoint;</t>
-  </si>
-  <si>
-    <t>http://www.sqlite.org/pragma.html#pragma_wal_autocheckpoint</t>
-  </si>
-  <si>
-    <t>"When the write-ahead log is enabled (via the journal_mode pragma) a checkpoint will be run automatically whenever the write-ahead log equals or exceeds N pages in length."</t>
-  </si>
-  <si>
-    <t>Positive value: Set cache to VALUE*page_size. Negative: Set cache directly to the value in kB (e.g. =-10 means 10 kB)</t>
-  </si>
-  <si>
-    <t>The following entries could also have an effect on performance but are not implemented by this program so far.</t>
-  </si>
-  <si>
-    <t>https://www.sqlite.org/lang_corefunc.html#sqlite_version</t>
-  </si>
-  <si>
-    <t>select sqlite_version();</t>
-  </si>
-  <si>
-    <t>?? BinaryGUID</t>
-  </si>
-  <si>
-    <t>?? Enlist</t>
-  </si>
-  <si>
-    <t>?? Cache Spill</t>
-  </si>
-  <si>
-    <t>?? Jounal Size Limit</t>
-  </si>
-  <si>
-    <t>?? Threads</t>
-  </si>
-  <si>
-    <t>?? WAL Checkpoint</t>
-  </si>
-  <si>
-    <t>?? WAL AutoCheckPoint</t>
-  </si>
-  <si>
-    <t>"True - Store GUID columns in binary form; False - Store GUID columns as text "</t>
-  </si>
-  <si>
-    <t>Auto Vacuum</t>
-  </si>
-  <si>
-    <t>http://www.sqlite.org/pragma.html#pragma_auto_vacuum</t>
-  </si>
-  <si>
-    <t>None/Full. Can be changed for new databases only. Enabled a "Mini Vacuum" after deleting data. The value INCREMENTAL is not supported by this program.</t>
-  </si>
-  <si>
-    <t>PRAGMA main.auto_vacuum;</t>
-  </si>
-  <si>
-    <t>PRAGMA main.wal_checkpoint;</t>
-  </si>
-  <si>
-    <t>Is verifiable?</t>
-  </si>
-  <si>
-    <t>Apply to existing databases?</t>
-  </si>
-  <si>
-    <t>Persistent (stored in database file)</t>
-  </si>
-  <si>
-    <t>?? Cell Size Check</t>
-  </si>
-  <si>
-    <t>PRAGMA cell_size_check;</t>
-  </si>
-  <si>
-    <t>http://www.sqlite.org/pragma.html#pragma_cell_size_check</t>
-  </si>
-  <si>
-    <t>"The cell_size_check pragma enables or disables additional sanity checking on database b-tree pages as they are initially read from disk."</t>
-  </si>
-  <si>
-    <t>??? In-Memory Database</t>
-  </si>
-  <si>
-    <t>Returns the SQLite version. Can not be set.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Can only be changed when the database is empty (before the first CREATE TABLE statement. Min=512, Max=65536 </t>
-  </si>
-  <si>
-    <t>x UTF-8 or UTF16le Encoding</t>
-  </si>
-  <si>
-    <t>x Cache Size</t>
-  </si>
-  <si>
-    <t>x Page Size</t>
-  </si>
-  <si>
-    <t>x SQLite Version</t>
-  </si>
-  <si>
-    <t>x Secure Delete</t>
-  </si>
-  <si>
-    <t>x Temp Store</t>
+    <t>Secure Delete</t>
+  </si>
+  <si>
+    <t>Temp Store</t>
+  </si>
+  <si>
+    <t>SQLite Version</t>
   </si>
 </sst>
 </file>
@@ -699,10 +702,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -732,13 +735,13 @@
         <v>2</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>6</v>
@@ -767,7 +770,7 @@
         <v>11</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -793,12 +796,12 @@
         <v>5</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>25</v>
+        <v>102</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>22</v>
@@ -816,10 +819,10 @@
         <v>21</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -827,13 +830,13 @@
         <v>101</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>5</v>
@@ -845,47 +848,47 @@
         <v>11</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B6" t="s">
-        <v>32</v>
+        <v>94</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>48</v>
+        <v>88</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>49</v>
+        <v>89</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>21</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>45</v>
+        <v>5</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7" s="4" t="s">
+      <c r="D7" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>5</v>
@@ -894,102 +897,102 @@
         <v>21</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>84</v>
+        <v>36</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>87</v>
+        <v>37</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>85</v>
+        <v>40</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>21</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>86</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>11</v>
+        <v>98</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>21</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>52</v>
+        <v>103</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>53</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>21</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>11</v>
@@ -1001,159 +1004,159 @@
         <v>5</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>61</v>
+        <v>30</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D13" s="2"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D14" s="2"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>73</v>
+      <c r="F17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>83</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>15</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>15</v>
@@ -1165,47 +1168,47 @@
         <v>15</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>63</v>
+        <v>84</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>15</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>15</v>
@@ -1217,59 +1220,59 @@
         <v>15</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>69</v>
+        <v>30</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>70</v>
+        <v>4</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>71</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B25" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B25" t="s">
         <v>31</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>93</v>
+        <v>47</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>94</v>
+        <v>48</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>95</v>
+        <v>11</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1277,53 +1280,53 @@
         <v>96</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>31</v>
+        <v>83</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>4</v>
+        <v>81</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C29" s="4"/>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C27" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D26" r:id="rId1"/>
+    <hyperlink ref="D24" r:id="rId1"/>
     <hyperlink ref="D2" r:id="rId2" location="pragma_encoding"/>
-    <hyperlink ref="D18" r:id="rId3"/>
+    <hyperlink ref="D17" r:id="rId3"/>
     <hyperlink ref="D3" r:id="rId4" location="pragma_cache_size"/>
     <hyperlink ref="D4" r:id="rId5" location="pragma_synchronous"/>
     <hyperlink ref="D5" r:id="rId6" location="pragma_page_size"/>
-    <hyperlink ref="D19" r:id="rId7"/>
-    <hyperlink ref="D6" r:id="rId8" location="pragma_legacy_file_format"/>
+    <hyperlink ref="D18" r:id="rId7"/>
+    <hyperlink ref="D25" r:id="rId8" location="pragma_legacy_file_format"/>
     <hyperlink ref="D7" r:id="rId9" location="pragma_journal_mode"/>
-    <hyperlink ref="D9" r:id="rId10" location="pragma_automatic_index"/>
-    <hyperlink ref="D20" r:id="rId11" location="pragma_cache_spill"/>
-    <hyperlink ref="D21" r:id="rId12" location="pragma_journal_size_limit"/>
-    <hyperlink ref="D10" r:id="rId13" location="pragma_locking_mode"/>
-    <hyperlink ref="D11" r:id="rId14" location="pragma_secure_delete"/>
-    <hyperlink ref="D12" r:id="rId15" location="pragma_temp_store"/>
-    <hyperlink ref="D22" r:id="rId16" location="pragma_threads"/>
-    <hyperlink ref="D23" r:id="rId17" location="pragma_wal_checkpoint"/>
-    <hyperlink ref="D24" r:id="rId18" location="pragma_wal_autocheckpoint"/>
-    <hyperlink ref="D13" r:id="rId19" location="sqlite_version"/>
-    <hyperlink ref="D8" r:id="rId20" location="pragma_auto_vacuum"/>
-    <hyperlink ref="D25" r:id="rId21" location="pragma_cell_size_check"/>
+    <hyperlink ref="D8" r:id="rId10" location="pragma_automatic_index"/>
+    <hyperlink ref="D19" r:id="rId11" location="pragma_cache_spill"/>
+    <hyperlink ref="D20" r:id="rId12" location="pragma_journal_size_limit"/>
+    <hyperlink ref="D9" r:id="rId13" location="pragma_locking_mode"/>
+    <hyperlink ref="D10" r:id="rId14" location="pragma_secure_delete"/>
+    <hyperlink ref="D11" r:id="rId15" location="pragma_temp_store"/>
+    <hyperlink ref="D21" r:id="rId16" location="pragma_threads"/>
+    <hyperlink ref="D22" r:id="rId17" location="pragma_wal_checkpoint"/>
+    <hyperlink ref="D23" r:id="rId18" location="pragma_wal_autocheckpoint"/>
+    <hyperlink ref="D12" r:id="rId19" location="sqlite_version"/>
+    <hyperlink ref="D26" r:id="rId20" location="pragma_auto_vacuum"/>
+    <hyperlink ref="D6" r:id="rId21" location="pragma_cell_size_check"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId22"/>

</xml_diff>